<commit_message>
Added Fig. 4 (b)
</commit_message>
<xml_diff>
--- a/Figures/Figure 4.xlsx
+++ b/Figures/Figure 4.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Macintosh HD/Users/matthewkelly/Documents/Papers/Hierarchical HDM/Submission ver 2/Indirect-Associations/Figures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexkelly/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79866EF7-6525-9145-A606-6B5C77DC3B14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC9D40C-8B46-1D40-A458-3D37EF83A1E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{D0B40D0E-66CA-F547-A8B5-12285A91E0B5}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" activeTab="2" xr2:uid="{D0B40D0E-66CA-F547-A8B5-12285A91E0B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Chart1" sheetId="3" r:id="rId2"/>
+    <sheet name="Fig. 4 (a)" sheetId="3" r:id="rId2"/>
+    <sheet name="Fig. 4 (b)" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,13 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>104 unique part of speech tag combinations</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Level 1</t>
   </si>
@@ -51,21 +48,31 @@
   <si>
     <t>Level 4</t>
   </si>
+  <si>
+    <t>total words</t>
+  </si>
+  <si>
+    <t>HHM level</t>
+  </si>
+  <si>
+    <t>Fig 4 (a) POS tag set</t>
+  </si>
+  <si>
+    <t>Fig 4 (b) dominant POS tag</t>
+  </si>
+  <si>
+    <t>classes</t>
+  </si>
+  <si>
+    <t>chance</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -95,8 +102,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -174,7 +181,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$A$4</c:f>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -194,7 +201,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$4</c:f>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -343,6 +350,236 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15862110248649999"/>
+          <c:y val="4.36170185363743E-2"/>
+          <c:w val="0.7995115460351726"/>
+          <c:h val="0.81680852214722799"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Series1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Level 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Level 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Level 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Level 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.53086123764618098</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.62135379205626096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.61160393191081197</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58131543195077096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B084-AB4D-8940-CC994576B1E4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="623168328"/>
+        <c:axId val="623240616"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="623168328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>vector representations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="623240616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="623240616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.65000000000000013"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>classification</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> accuracy</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.3710842541218899E-2"/>
+              <c:y val="0.201674447038379"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="623168328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1.0000000000000002E-2"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="2000">
+          <a:latin typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{6A4EEE9D-31D7-304C-AAA4-C23490B76163}">
   <sheetPr/>
@@ -355,17 +592,62 @@
 </chartsheet>
 </file>
 
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{6E214D00-72DC-F043-9457-B5D5DF326E5F}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8685893" cy="6281964"/>
+    <xdr:ext cx="8685893" cy="6293304"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C7127B9-DF31-8049-9EFF-B9A7EA9FC1BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8685893" cy="6293304"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C48DC4A5-A59B-FF4B-B1EC-1C83258EEC2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -685,57 +967,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D8CA1B-5CCB-C247-9EE4-253153B565DA}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.20152891351250499</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.53086123764618098</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.22068028660469299</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.62135379205626096</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2">
-        <v>0.20152891351250499</v>
+      <c r="B4" s="1">
+        <v>0.22568787790000799</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.61160393191081197</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.22068028660469299</v>
+      <c r="B5" s="1">
+        <v>0.19497642703033799</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.58131543195077096</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.22568787790000799</v>
+      <c r="B6">
+        <v>37543</v>
+      </c>
+      <c r="C6">
+        <v>37539</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.19497642703033799</v>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>104</v>
+      </c>
+      <c r="C7">
+        <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>37543</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <f>1/B7</f>
+        <v>9.6153846153846159E-3</v>
+      </c>
+      <c r="C8" s="1">
+        <f>1/C7</f>
+        <v>3.4482758620689655E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>